<commit_message>
Removed pin2 pullup resistor. Uploaded and updated files for Rev3B.
</commit_message>
<xml_diff>
--- a/generated/barnabas_noggin_V4_ListByValues.xlsx
+++ b/generated/barnabas_noggin_V4_ListByValues.xlsx
@@ -1,29 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ling\Desktop\Barnabas\barnabas-noggin\generated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDD92521-5586-4AD0-B34B-CB86AED644DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A78BBDDB-A125-48FC-9F3B-3CEE5A1B5B56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276"/>
   </bookViews>
   <sheets>
     <sheet name="barnabas_noggin_V4_ListByValues" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -72,7 +64,7 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R1, R4, R5, R6, R7, R8, R9, R10</t>
+    <t>R1, R4, R5, R6, R7, R8, R9</t>
   </si>
   <si>
     <t>Yageo</t>
@@ -1413,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1466,7 +1458,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2410,6 +2402,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>